<commit_message>
Add new actions: 	- AbstractAction::Action_BlockOneEnemyAttackForOneTurn 	- AbstractAction::Action_EnemyCanAttackOnNextTurn_Random 	- AbstractAction::Action_UniqueAttack_Random Handle blocking attacks
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2396,9 +2397,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="B1:CB204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -23462,8 +23463,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="B1:L103"/>
   <sheetViews>
-    <sheetView topLeftCell="G47" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView topLeftCell="G50" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Correction of minors bugs
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -19,7 +19,6 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -859,9 +858,6 @@
     <t>Mania</t>
   </si>
   <si>
-    <t>Lancez une pièce. Si c'est face, cette attaque inflige 30 dégâts plus 10 dégâts supplémentaires ; si c'est pile, cette attaque inflige 30 dégâts et Nidoking s'inflige 10 dégâts.</t>
-  </si>
-  <si>
     <t>Toxik</t>
   </si>
   <si>
@@ -1009,9 +1005,6 @@
     <t>Poing-éclair</t>
   </si>
   <si>
-    <t>Lancez une pièce. Si c'est face, cette attaque inflige 30 dégâts plus 10 dégâts supplémentaires ; si c'est pile, cette attaque inflige 30 dégâts et Élektek s'inflige 10 dégâts.</t>
-  </si>
-  <si>
     <t>Draco-rage</t>
   </si>
   <si>
@@ -1340,9 +1333,6 @@
   </si>
   <si>
     <t>Gaz infect</t>
-  </si>
-  <si>
-    <t>Lancez une pièce. Si c'est face, le Pokémon Défenseur est maintenant Empoisonné ; si c'est pile, il est maintenant Confus.</t>
   </si>
   <si>
     <t>Balayage</t>
@@ -1796,6 +1786,15 @@
   </si>
   <si>
     <t>Coef faib</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, cette attaque inflige 30 dégâts plus 10 dégâts supplémentaires , si c'est pile, cette attaque inflige 30 dégâts et Nidoking s'inflige 10 dégâts.</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, le Pokémon Défenseur est maintenant Empoisonné , si c'est pile, il est maintenant Confus.</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, cette attaque inflige 30 dégâts plus 10 dégâts supplémentaires , si c'est pile, cette attaque inflige 30 dégâts et Élektek s'inflige 10 dégâts.</t>
   </si>
 </sst>
 </file>
@@ -2397,9 +2396,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="B1:CB204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK110" sqref="AK110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2612,7 +2611,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>0</v>
@@ -2630,13 +2629,13 @@
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>191</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>190</v>
@@ -2654,7 +2653,7 @@
         <v>193</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>222</v>
@@ -2705,10 +2704,10 @@
         <v>12</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AJ4" s="5" t="s">
         <v>0</v>
@@ -2720,7 +2719,7 @@
         <v>193</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AN4" s="1" t="s">
         <v>222</v>
@@ -2771,10 +2770,10 @@
         <v>12</v>
       </c>
       <c r="BD4" s="4" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="BE4" s="4" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="BF4" s="6" t="s">
         <v>0</v>
@@ -3878,7 +3877,7 @@
         <v>40</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -4464,7 +4463,7 @@
         <v>218</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -4601,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AB19">
         <v>3</v>
@@ -4703,7 +4702,7 @@
         <v>268</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="P20" s="1">
         <v>10</v>
@@ -4822,7 +4821,7 @@
         <v>268</v>
       </c>
       <c r="O21" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="P21">
         <v>10</v>
@@ -5156,16 +5155,16 @@
       <c r="AG24" s="1"/>
       <c r="AH24" s="7"/>
       <c r="AJ24" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AK24" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AL24" s="1">
         <v>0</v>
       </c>
       <c r="AM24" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
@@ -5636,7 +5635,7 @@
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1">
@@ -5666,10 +5665,10 @@
       <c r="AG29" s="1"/>
       <c r="AH29" s="7"/>
       <c r="AJ29" s="5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="AK29" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="AL29" s="1">
         <v>30</v>
@@ -5872,10 +5871,10 @@
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="6" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="P31" s="1">
         <v>10</v>
@@ -6371,10 +6370,10 @@
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>
@@ -6490,7 +6489,7 @@
         <v>32</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>266</v>
@@ -6499,7 +6498,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -6530,7 +6529,7 @@
         <v>2</v>
       </c>
       <c r="AJ37" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AK37" s="5"/>
       <c r="AL37" s="1">
@@ -6620,13 +6619,13 @@
         <v>275</v>
       </c>
       <c r="O38" t="s">
-        <v>276</v>
+        <v>583</v>
       </c>
       <c r="P38">
         <v>30</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="Z38">
         <v>1</v>
@@ -6644,10 +6643,10 @@
         <v>10</v>
       </c>
       <c r="AJ38" t="s">
+        <v>276</v>
+      </c>
+      <c r="AK38" t="s">
         <v>277</v>
-      </c>
-      <c r="AK38" t="s">
-        <v>278</v>
       </c>
       <c r="AL38">
         <v>20</v>
@@ -6722,10 +6721,10 @@
       </c>
       <c r="M39" s="4"/>
       <c r="N39" t="s">
+        <v>278</v>
+      </c>
+      <c r="O39" t="s">
         <v>279</v>
-      </c>
-      <c r="O39" t="s">
-        <v>280</v>
       </c>
       <c r="P39">
         <v>0</v>
@@ -6747,10 +6746,10 @@
         <v>-1</v>
       </c>
       <c r="AJ39" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK39" t="s">
         <v>281</v>
-      </c>
-      <c r="AK39" t="s">
-        <v>282</v>
       </c>
       <c r="AL39">
         <v>0</v>
@@ -7036,10 +7035,10 @@
         <v>37</v>
       </c>
       <c r="N42" t="s">
+        <v>282</v>
+      </c>
+      <c r="O42" t="s">
         <v>283</v>
-      </c>
-      <c r="O42" t="s">
-        <v>284</v>
       </c>
       <c r="P42">
         <v>0</v>
@@ -7055,10 +7054,10 @@
         <v>702</v>
       </c>
       <c r="AJ42" t="s">
+        <v>284</v>
+      </c>
+      <c r="AK42" t="s">
         <v>285</v>
-      </c>
-      <c r="AK42" t="s">
-        <v>286</v>
       </c>
       <c r="AL42">
         <v>80</v>
@@ -8194,7 +8193,7 @@
       </c>
       <c r="M54" s="4"/>
       <c r="N54" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O54" s="1"/>
       <c r="P54" s="1">
@@ -8224,7 +8223,7 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="7"/>
       <c r="AJ54" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AK54" s="5"/>
       <c r="AL54" s="1">
@@ -8328,10 +8327,10 @@
         <v>1</v>
       </c>
       <c r="AJ55" t="s">
+        <v>286</v>
+      </c>
+      <c r="AK55" t="s">
         <v>287</v>
-      </c>
-      <c r="AK55" t="s">
-        <v>288</v>
       </c>
       <c r="AL55">
         <v>70</v>
@@ -8979,7 +8978,7 @@
       </c>
       <c r="M62" s="4"/>
       <c r="N62" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P62">
         <v>20</v>
@@ -9077,7 +9076,7 @@
         <v>201</v>
       </c>
       <c r="O63" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P63">
         <v>50</v>
@@ -9102,10 +9101,10 @@
         <v>5</v>
       </c>
       <c r="AJ63" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK63" t="s">
         <v>291</v>
-      </c>
-      <c r="AK63" t="s">
-        <v>292</v>
       </c>
       <c r="AL63">
         <v>80</v>
@@ -9182,16 +9181,16 @@
       </c>
       <c r="M64" s="4"/>
       <c r="N64" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="P64" s="1">
         <v>30</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
@@ -9301,10 +9300,10 @@
         <v>60</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P65" s="1">
         <v>0</v>
@@ -9335,7 +9334,7 @@
       </c>
       <c r="AH65" s="7"/>
       <c r="AJ65" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AK65" s="5" t="s">
         <v>266</v>
@@ -9344,7 +9343,7 @@
         <v>0</v>
       </c>
       <c r="AM65" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AN65" s="1"/>
       <c r="AO65" s="1"/>
@@ -9430,16 +9429,16 @@
         <v>61</v>
       </c>
       <c r="N66" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O66" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="P66">
         <v>30</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="AB66">
         <v>1</v>
@@ -9457,10 +9456,10 @@
         <v>0</v>
       </c>
       <c r="AJ66" t="s">
+        <v>293</v>
+      </c>
+      <c r="AK66" t="s">
         <v>294</v>
-      </c>
-      <c r="AK66" t="s">
-        <v>295</v>
       </c>
       <c r="AL66">
         <v>40</v>
@@ -9540,10 +9539,10 @@
       </c>
       <c r="M67" s="4"/>
       <c r="N67" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P67" s="1">
         <v>10</v>
@@ -9663,7 +9662,7 @@
         <v>253</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="P68" s="1">
         <v>0</v>
@@ -9699,7 +9698,7 @@
         <v>12</v>
       </c>
       <c r="AJ68" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AK68" s="5"/>
       <c r="AL68" s="1">
@@ -9870,10 +9869,10 @@
       <c r="BW69" s="1"/>
       <c r="BX69" s="4"/>
       <c r="BY69" t="s">
+        <v>295</v>
+      </c>
+      <c r="BZ69" t="s">
         <v>296</v>
-      </c>
-      <c r="BZ69" t="s">
-        <v>297</v>
       </c>
       <c r="CA69" s="1"/>
       <c r="CB69" s="7"/>
@@ -9910,7 +9909,7 @@
       </c>
       <c r="M70" s="4"/>
       <c r="N70" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="O70" s="1"/>
       <c r="P70" s="1">
@@ -10021,16 +10020,16 @@
         <v>66</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="P71" s="1">
         <v>0</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
@@ -10061,10 +10060,10 @@
         <v>10</v>
       </c>
       <c r="AJ71" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AK71" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AL71" s="1">
         <v>60</v>
@@ -10154,7 +10153,7 @@
         <v>67</v>
       </c>
       <c r="N72" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P72">
         <v>60</v>
@@ -10213,10 +10212,10 @@
       <c r="BW72" s="1"/>
       <c r="BX72" s="4"/>
       <c r="BY72" t="s">
+        <v>297</v>
+      </c>
+      <c r="BZ72" t="s">
         <v>298</v>
-      </c>
-      <c r="BZ72" t="s">
-        <v>299</v>
       </c>
       <c r="CA72" s="1"/>
       <c r="CB72" s="7"/>
@@ -11427,10 +11426,10 @@
       </c>
       <c r="M85" s="4"/>
       <c r="N85" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="O85" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="O85" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="P85" s="1">
         <v>10</v>
@@ -11466,10 +11465,10 @@
         <v>-1</v>
       </c>
       <c r="AJ85" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AK85" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="AL85" s="1">
         <v>40</v>
@@ -11559,10 +11558,10 @@
         <v>81</v>
       </c>
       <c r="N86" t="s">
+        <v>300</v>
+      </c>
+      <c r="O86" t="s">
         <v>301</v>
-      </c>
-      <c r="O86" t="s">
-        <v>302</v>
       </c>
       <c r="P86">
         <v>30</v>
@@ -11587,10 +11586,10 @@
         <v>-1</v>
       </c>
       <c r="AJ86" t="s">
+        <v>302</v>
+      </c>
+      <c r="AK86" t="s">
         <v>303</v>
-      </c>
-      <c r="AK86" t="s">
-        <v>304</v>
       </c>
       <c r="AL86">
         <v>80</v>
@@ -11668,10 +11667,10 @@
       </c>
       <c r="M87" s="4"/>
       <c r="N87" t="s">
+        <v>304</v>
+      </c>
+      <c r="O87" t="s">
         <v>305</v>
-      </c>
-      <c r="O87" t="s">
-        <v>306</v>
       </c>
       <c r="P87">
         <v>30</v>
@@ -11687,7 +11686,7 @@
         <v>102</v>
       </c>
       <c r="AJ87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AL87">
         <v>30</v>
@@ -11757,16 +11756,16 @@
       </c>
       <c r="M88" s="4"/>
       <c r="N88" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P88" s="1">
         <v>0</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
@@ -11971,7 +11970,7 @@
       </c>
       <c r="M90" s="4"/>
       <c r="N90" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="O90" s="1"/>
       <c r="P90" s="1">
@@ -12080,7 +12079,7 @@
         <v>86</v>
       </c>
       <c r="N91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P91">
         <v>30</v>
@@ -12096,10 +12095,10 @@
         <v>2</v>
       </c>
       <c r="AJ91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AK91" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AL91">
         <v>50</v>
@@ -12563,10 +12562,10 @@
       </c>
       <c r="M96" s="4"/>
       <c r="N96" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P96" s="1">
         <v>0</v>
@@ -12602,10 +12601,10 @@
         <v>-1</v>
       </c>
       <c r="AJ96" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AK96" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AL96" s="1">
         <v>0</v>
@@ -12697,10 +12696,10 @@
         <v>92</v>
       </c>
       <c r="N97" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="P97" s="1">
         <v>0</v>
@@ -12733,10 +12732,10 @@
         <v>4</v>
       </c>
       <c r="AJ97" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AK97" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AL97" s="1">
         <v>0</v>
@@ -12920,7 +12919,7 @@
       </c>
       <c r="M99" s="4"/>
       <c r="N99" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="O99" s="1"/>
       <c r="P99" s="1">
@@ -12953,7 +12952,7 @@
         <v>218</v>
       </c>
       <c r="AK99" s="5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="AL99" s="1">
         <v>0</v>
@@ -13041,7 +13040,7 @@
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="O100" s="1"/>
       <c r="P100" s="1">
@@ -13071,10 +13070,10 @@
       <c r="AG100" s="1"/>
       <c r="AH100" s="7"/>
       <c r="AJ100" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AK100" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AL100" s="1">
         <v>0</v>
@@ -13561,10 +13560,10 @@
         <v>100</v>
       </c>
       <c r="N105" t="s">
+        <v>311</v>
+      </c>
+      <c r="O105" t="s">
         <v>312</v>
-      </c>
-      <c r="O105" t="s">
-        <v>313</v>
       </c>
       <c r="P105">
         <v>50</v>
@@ -13629,10 +13628,10 @@
       <c r="BW105" s="1"/>
       <c r="BX105" s="4"/>
       <c r="BY105" t="s">
+        <v>309</v>
+      </c>
+      <c r="BZ105" t="s">
         <v>310</v>
-      </c>
-      <c r="BZ105" t="s">
-        <v>311</v>
       </c>
       <c r="CA105" s="1"/>
       <c r="CB105" s="7"/>
@@ -14146,7 +14145,7 @@
       </c>
       <c r="M111" s="4"/>
       <c r="N111" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P111">
         <v>20</v>
@@ -14159,7 +14158,7 @@
         <v>1</v>
       </c>
       <c r="AJ111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL111">
         <v>40</v>
@@ -14326,10 +14325,10 @@
       </c>
       <c r="M113" s="4"/>
       <c r="N113" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="O113" s="1" t="s">
-        <v>437</v>
+        <v>584</v>
       </c>
       <c r="P113" s="1">
         <v>10</v>
@@ -14734,10 +14733,10 @@
       </c>
       <c r="M117" s="4"/>
       <c r="N117" t="s">
+        <v>315</v>
+      </c>
+      <c r="O117" t="s">
         <v>316</v>
-      </c>
-      <c r="O117" t="s">
-        <v>317</v>
       </c>
       <c r="P117">
         <v>0</v>
@@ -14753,10 +14752,10 @@
         <v>500</v>
       </c>
       <c r="AJ117" t="s">
+        <v>317</v>
+      </c>
+      <c r="AK117" t="s">
         <v>318</v>
-      </c>
-      <c r="AK117" t="s">
-        <v>319</v>
       </c>
       <c r="AL117">
         <v>80</v>
@@ -15875,16 +15874,16 @@
       </c>
       <c r="M128" s="4"/>
       <c r="N128" t="s">
+        <v>319</v>
+      </c>
+      <c r="O128" t="s">
         <v>320</v>
       </c>
-      <c r="O128" t="s">
-        <v>321</v>
-      </c>
       <c r="P128">
         <v>0</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="AD128">
         <v>1</v>
@@ -15899,16 +15898,16 @@
         <v>2</v>
       </c>
       <c r="AJ128" t="s">
+        <v>321</v>
+      </c>
+      <c r="AK128" t="s">
         <v>322</v>
-      </c>
-      <c r="AK128" t="s">
-        <v>323</v>
       </c>
       <c r="AL128">
         <v>20</v>
       </c>
       <c r="AM128" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="AX128">
         <v>1</v>
@@ -15976,10 +15975,10 @@
       </c>
       <c r="M129" s="4"/>
       <c r="N129" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O129" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P129">
         <v>10</v>
@@ -16001,16 +16000,16 @@
         <v>-1</v>
       </c>
       <c r="AJ129" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AK129" t="s">
-        <v>326</v>
+        <v>585</v>
       </c>
       <c r="AL129">
         <v>30</v>
       </c>
       <c r="AM129" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="AQ129">
         <v>1</v>
@@ -16083,7 +16082,7 @@
       </c>
       <c r="M130" s="4"/>
       <c r="N130" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="O130" s="1"/>
       <c r="P130" s="1">
@@ -16116,7 +16115,7 @@
         <v>201</v>
       </c>
       <c r="AK130" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AL130" s="1">
         <v>50</v>
@@ -16429,16 +16428,16 @@
       <c r="AG133" s="1"/>
       <c r="AH133" s="7"/>
       <c r="AJ133" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AK133" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AL133" s="1">
         <v>0</v>
       </c>
       <c r="AM133" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="AN133" s="1"/>
       <c r="AO133" s="1"/>
@@ -16522,7 +16521,7 @@
         <v>129</v>
       </c>
       <c r="N134" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P134">
         <v>50</v>
@@ -16535,10 +16534,10 @@
         <v>3</v>
       </c>
       <c r="AJ134" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AK134" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AL134">
         <v>40</v>
@@ -17193,10 +17192,10 @@
       </c>
       <c r="M141" s="4"/>
       <c r="N141" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="P141" s="1">
         <v>0</v>
@@ -17227,10 +17226,10 @@
       </c>
       <c r="AH141" s="7"/>
       <c r="AJ141" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AK141" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AL141" s="1"/>
       <c r="AM141" s="1">
@@ -17981,10 +17980,10 @@
       </c>
       <c r="M149" s="4"/>
       <c r="N149" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O149" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P149">
         <v>60</v>
@@ -18009,10 +18008,10 @@
         <v>30</v>
       </c>
       <c r="AJ149" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AK149" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AL149">
         <v>100</v>
@@ -18136,7 +18135,7 @@
       </c>
       <c r="M151" s="4"/>
       <c r="N151" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P151">
         <v>10</v>
@@ -18208,7 +18207,7 @@
         <v>147</v>
       </c>
       <c r="N152" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O152" t="s">
         <v>266</v>
@@ -18217,7 +18216,7 @@
         <v>0</v>
       </c>
       <c r="Q152" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AB152">
         <v>3</v>
@@ -18232,10 +18231,10 @@
         <v>2</v>
       </c>
       <c r="AJ152" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AK152" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AL152">
         <v>20</v>
@@ -18361,16 +18360,16 @@
       </c>
       <c r="M154" s="4"/>
       <c r="N154" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O154" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P154">
         <v>10</v>
       </c>
       <c r="Q154" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="AB154">
         <v>1</v>
@@ -18388,10 +18387,10 @@
         <v>0</v>
       </c>
       <c r="AJ154" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AK154" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AL154">
         <v>0</v>
@@ -22562,16 +22561,16 @@
         <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -22857,7 +22856,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>0</v>
@@ -22866,10 +22865,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>342</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -22880,10 +22879,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F3" s="6">
         <v>2000</v>
@@ -22898,10 +22897,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F4" s="6">
         <v>2001</v>
@@ -22916,10 +22915,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F5" s="6">
         <v>2002</v>
@@ -22934,10 +22933,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F6" s="6">
         <v>2003</v>
@@ -22952,10 +22951,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F7" s="6">
         <v>2004</v>
@@ -22970,10 +22969,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F8" s="6">
         <v>2005</v>
@@ -22988,10 +22987,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F9" s="6">
         <v>2006</v>
@@ -23006,10 +23005,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F10" s="6">
         <v>2007</v>
@@ -23024,10 +23023,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F11" s="6">
         <v>2008</v>
@@ -23042,10 +23041,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F12" s="6">
         <v>2009</v>
@@ -23060,10 +23059,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F13" s="6">
         <v>2010</v>
@@ -23078,10 +23077,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F14" s="6">
         <v>2011</v>
@@ -23096,10 +23095,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F15" s="6">
         <v>2012</v>
@@ -23114,10 +23113,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F16" s="6">
         <v>2013</v>
@@ -23132,10 +23131,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F17" s="6">
         <v>2014</v>
@@ -23150,10 +23149,10 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F18" s="6">
         <v>2015</v>
@@ -23168,10 +23167,10 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F19" s="6">
         <v>2016</v>
@@ -23186,10 +23185,10 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F20" s="6">
         <v>2017</v>
@@ -23204,10 +23203,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F21" s="6">
         <v>2018</v>
@@ -23222,10 +23221,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E22" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F22" s="6">
         <v>2019</v>
@@ -23240,10 +23239,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F23" s="6">
         <v>2020</v>
@@ -23258,10 +23257,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F24" s="6">
         <v>2021</v>
@@ -23276,10 +23275,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F25" s="6">
         <v>2022</v>
@@ -23294,10 +23293,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F26" s="6">
         <v>2023</v>
@@ -23312,10 +23311,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F27" s="6">
         <v>2024</v>
@@ -23330,10 +23329,10 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F28" s="6">
         <v>2025</v>
@@ -23478,7 +23477,7 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="2:10">
@@ -23497,16 +23496,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="I4" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -23520,10 +23519,10 @@
         <v>4</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I5" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -23537,10 +23536,10 @@
         <v>5</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -23554,10 +23553,10 @@
         <v>6</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -23571,10 +23570,10 @@
         <v>7</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I8" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="J8">
         <v>4</v>
@@ -23588,10 +23587,10 @@
         <v>8</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I9" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="J9">
         <v>5</v>
@@ -23605,10 +23604,10 @@
         <v>9</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J10">
         <v>6</v>
@@ -23622,10 +23621,10 @@
         <v>10</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I11" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="J11">
         <v>7</v>
@@ -23639,10 +23638,10 @@
         <v>11</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="I12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J12">
         <v>8</v>
@@ -23650,10 +23649,10 @@
     </row>
     <row r="13" spans="2:10">
       <c r="H13" s="22" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I13" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="J13">
         <v>9</v>
@@ -23661,10 +23660,10 @@
     </row>
     <row r="14" spans="2:10">
       <c r="H14" s="22" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="J14">
         <v>10</v>
@@ -23672,10 +23671,10 @@
     </row>
     <row r="15" spans="2:10">
       <c r="H15" s="22" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I15" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="J15">
         <v>11</v>
@@ -23683,10 +23682,10 @@
     </row>
     <row r="16" spans="2:10">
       <c r="H16" s="22" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I16" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J16">
         <v>12</v>
@@ -23694,10 +23693,10 @@
     </row>
     <row r="17" spans="8:10">
       <c r="H17" s="22" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I17" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="J17">
         <v>13</v>
@@ -23705,10 +23704,10 @@
     </row>
     <row r="18" spans="8:10">
       <c r="H18" s="22" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="J18">
         <v>14</v>
@@ -23716,10 +23715,10 @@
     </row>
     <row r="19" spans="8:10">
       <c r="H19" s="22" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J19">
         <v>15</v>
@@ -23727,10 +23726,10 @@
     </row>
     <row r="20" spans="8:10">
       <c r="H20" s="22" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I20" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J20">
         <v>16</v>
@@ -23738,10 +23737,10 @@
     </row>
     <row r="21" spans="8:10">
       <c r="H21" s="22" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I21" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="J21">
         <v>17</v>
@@ -23749,10 +23748,10 @@
     </row>
     <row r="22" spans="8:10">
       <c r="H22" s="22" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I22" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J22">
         <v>18</v>
@@ -23760,10 +23759,10 @@
     </row>
     <row r="23" spans="8:10">
       <c r="H23" s="22" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I23" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J23">
         <v>19</v>
@@ -23771,10 +23770,10 @@
     </row>
     <row r="24" spans="8:10">
       <c r="H24" s="22" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I24" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="J24">
         <v>20</v>
@@ -23782,10 +23781,10 @@
     </row>
     <row r="25" spans="8:10">
       <c r="H25" s="22" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I25" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="J25">
         <v>21</v>
@@ -23793,10 +23792,10 @@
     </row>
     <row r="26" spans="8:10">
       <c r="H26" s="22" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I26" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J26">
         <v>22</v>
@@ -23804,10 +23803,10 @@
     </row>
     <row r="27" spans="8:10">
       <c r="H27" s="22" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="J27">
         <v>23</v>
@@ -23815,10 +23814,10 @@
     </row>
     <row r="28" spans="8:10">
       <c r="H28" s="22" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I28" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J28">
         <v>24</v>
@@ -23826,10 +23825,10 @@
     </row>
     <row r="29" spans="8:10">
       <c r="H29" s="22" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I29" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="J29">
         <v>25</v>
@@ -23837,10 +23836,10 @@
     </row>
     <row r="30" spans="8:10">
       <c r="H30" s="22" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I30" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="J30">
         <v>26</v>
@@ -23848,10 +23847,10 @@
     </row>
     <row r="31" spans="8:10">
       <c r="H31" s="22" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I31" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="J31">
         <v>27</v>
@@ -23859,10 +23858,10 @@
     </row>
     <row r="32" spans="8:10">
       <c r="H32" s="22" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I32" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="J32">
         <v>28</v>
@@ -23870,10 +23869,10 @@
     </row>
     <row r="33" spans="7:11">
       <c r="H33" s="22" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="J33">
         <v>29</v>
@@ -23881,10 +23880,10 @@
     </row>
     <row r="34" spans="7:11">
       <c r="H34" s="22" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I34" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="J34">
         <v>30</v>
@@ -23892,10 +23891,10 @@
     </row>
     <row r="35" spans="7:11">
       <c r="H35" s="22" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I35" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="J35">
         <v>31</v>
@@ -23903,10 +23902,10 @@
     </row>
     <row r="36" spans="7:11">
       <c r="H36" s="22" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I36" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="J36">
         <v>32</v>
@@ -23914,10 +23913,10 @@
     </row>
     <row r="37" spans="7:11">
       <c r="H37" s="22" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J37">
         <v>33</v>
@@ -23925,10 +23924,10 @@
     </row>
     <row r="38" spans="7:11">
       <c r="H38" s="22" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I38" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="J38">
         <v>34</v>
@@ -23936,10 +23935,10 @@
     </row>
     <row r="39" spans="7:11">
       <c r="H39" s="22" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I39" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="J39">
         <v>35</v>
@@ -23947,10 +23946,10 @@
     </row>
     <row r="40" spans="7:11">
       <c r="H40" s="22" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I40" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="J40">
         <v>36</v>
@@ -23958,10 +23957,10 @@
     </row>
     <row r="41" spans="7:11">
       <c r="H41" s="22" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I41" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="J41">
         <v>37</v>
@@ -23969,10 +23968,10 @@
     </row>
     <row r="42" spans="7:11">
       <c r="H42" s="22" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I42" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="J42">
         <v>38</v>
@@ -23980,10 +23979,10 @@
     </row>
     <row r="43" spans="7:11">
       <c r="H43" s="23" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I43" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="J43">
         <v>39</v>
@@ -23991,10 +23990,10 @@
     </row>
     <row r="46" spans="7:11">
       <c r="G46" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H46" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -24002,35 +24001,35 @@
     </row>
     <row r="47" spans="7:11">
       <c r="H47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I47">
         <v>1</v>
       </c>
       <c r="K47" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="48" spans="7:11">
       <c r="H48" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="I48">
         <v>2</v>
       </c>
       <c r="K48" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="49" spans="7:11">
       <c r="H49" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I49">
         <v>3</v>
       </c>
       <c r="K49" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="50" spans="7:11">
@@ -24038,10 +24037,10 @@
     </row>
     <row r="52" spans="7:11">
       <c r="G52" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H52" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="I52">
         <v>100</v>
@@ -24049,7 +24048,7 @@
     </row>
     <row r="53" spans="7:11">
       <c r="H53" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I53">
         <v>101</v>
@@ -24057,29 +24056,29 @@
     </row>
     <row r="54" spans="7:11">
       <c r="H54" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I54">
         <v>102</v>
       </c>
       <c r="K54" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="55" spans="7:11">
       <c r="H55" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="I55">
         <v>103</v>
       </c>
       <c r="K55" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="56" spans="7:11">
       <c r="H56" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I56">
         <v>104</v>
@@ -24087,18 +24086,18 @@
     </row>
     <row r="57" spans="7:11">
       <c r="H57" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I57">
         <v>105</v>
       </c>
       <c r="K57" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="58" spans="7:11">
       <c r="H58" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="I58">
         <v>106</v>
@@ -24106,7 +24105,7 @@
     </row>
     <row r="60" spans="7:11">
       <c r="G60" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="61" spans="7:11">
@@ -24120,74 +24119,74 @@
     </row>
     <row r="66" spans="7:12">
       <c r="G66" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H66" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I66">
         <v>200</v>
       </c>
       <c r="K66" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="L66" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="67" spans="7:12">
       <c r="H67" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="I67">
         <v>201</v>
       </c>
       <c r="K67" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="L67" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="68" spans="7:12">
       <c r="H68" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I68">
         <v>202</v>
       </c>
       <c r="K68" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="69" spans="7:12">
       <c r="H69" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I69">
         <v>203</v>
       </c>
       <c r="K69" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="70" spans="7:12">
       <c r="H70" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I70">
         <v>204</v>
       </c>
       <c r="K70" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="L70" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="71" spans="7:12">
       <c r="H71" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="I71">
         <v>205</v>
@@ -24195,94 +24194,94 @@
     </row>
     <row r="72" spans="7:12">
       <c r="H72" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I72">
         <v>206</v>
       </c>
       <c r="K72" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="73" spans="7:12">
       <c r="H73" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I73">
         <v>207</v>
       </c>
       <c r="K73" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="L73" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="74" spans="7:12">
       <c r="H74" s="20" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I74">
         <v>208</v>
       </c>
       <c r="K74" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="L74" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="76" spans="7:12">
       <c r="G76" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="H76" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I76">
         <v>300</v>
       </c>
       <c r="K76" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="L76" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="77" spans="7:12">
       <c r="H77" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I77">
         <v>301</v>
       </c>
       <c r="K77" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="L77" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="83" spans="7:12">
       <c r="G83" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H83" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I83">
         <v>400</v>
       </c>
       <c r="K83" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="L83" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="84" spans="7:12">
       <c r="H84" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I84">
         <v>401</v>
@@ -24290,10 +24289,10 @@
     </row>
     <row r="89" spans="7:12">
       <c r="G89" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H89" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I89">
         <v>500</v>
@@ -24301,7 +24300,7 @@
     </row>
     <row r="90" spans="7:12">
       <c r="H90" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I90">
         <v>501</v>
@@ -24309,93 +24308,93 @@
     </row>
     <row r="91" spans="7:12">
       <c r="H91" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I91">
         <v>502</v>
       </c>
       <c r="K91" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="92" spans="7:12">
       <c r="H92" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="I92">
         <v>503</v>
       </c>
       <c r="K92" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="95" spans="7:12">
       <c r="G95" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H95" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I95">
         <v>600</v>
       </c>
       <c r="K95" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="96" spans="7:12">
       <c r="H96" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I96">
         <v>601</v>
       </c>
       <c r="K96" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="L96" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="97" spans="7:11">
       <c r="H97" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="I97">
         <v>602</v>
       </c>
       <c r="K97" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="101" spans="7:11">
       <c r="G101" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H101" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="I101">
         <v>700</v>
       </c>
       <c r="K101" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="102" spans="7:11">
       <c r="H102" s="20" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="I102">
         <v>701</v>
       </c>
       <c r="K102" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="103" spans="7:11">
       <c r="H103" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="I103">
         <v>702</v>

</xml_diff>

<commit_message>
Rework on displays and move among packets Do not take index anymore but AbstractCard* Correction of minor bugs Add new action: - AbstractAction::Action_CompleteProtectionRandom Update database
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon" sheetId="1" r:id="rId1"/>
@@ -2396,9 +2396,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="B1:CB204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK110" sqref="AK110"/>
+    <sheetView topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH30" sqref="AH30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5767,11 +5767,10 @@
         <v>272</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q30" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U30">
         <v>1</v>
@@ -5780,10 +5779,7 @@
         <v>2</v>
       </c>
       <c r="AG30">
-        <v>502</v>
-      </c>
-      <c r="AH30">
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="AJ30" t="s">
         <v>273</v>
@@ -22839,8 +22835,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22894,7 +22890,7 @@
         <v>2001</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>348</v>
@@ -22948,7 +22944,7 @@
         <v>2004</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>351</v>
@@ -23074,7 +23070,7 @@
         <v>2011</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>368</v>
@@ -23146,7 +23142,7 @@
         <v>2015</v>
       </c>
       <c r="C18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>374</v>
@@ -23272,7 +23268,7 @@
         <v>2022</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>385</v>

</xml_diff>